<commit_message>
Added data provider to AdvancedResultsLoad
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-cts.xlsx
+++ b/test-data/webanalytics-cts.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFD67E3E-8BC4-4FDF-8245-846076AB78AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1DC2209E-C06F-4FEB-8D03-CB5930E1230A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DynamicListingPage" sheetId="9" r:id="rId1"/>
+    <sheet name="AdvancedResultsLoad" sheetId="10" r:id="rId1"/>
+    <sheet name="BasicResultsLoad" sheetId="11" r:id="rId2"/>
+    <sheet name="DynamicListingPage" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
   <si>
     <t>Path</t>
   </si>
@@ -79,6 +81,285 @@
   </si>
   <si>
     <t>manual parameters|</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>All Trials</t>
+  </si>
+  <si>
+    <t>Cancer Type</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Location (VA)</t>
+  </si>
+  <si>
+    <t>Location (NIH)</t>
+  </si>
+  <si>
+    <t>Location (Zip)</t>
+  </si>
+  <si>
+    <t>Location (City)</t>
+  </si>
+  <si>
+    <t>Location (Hospital)</t>
+  </si>
+  <si>
+    <t>Trial Type</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Trial ID</t>
+  </si>
+  <si>
+    <t>Investigator</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Kitchen Sink</t>
+  </si>
+  <si>
+    <t>SearchType</t>
+  </si>
+  <si>
+    <t>CtsFieldsUsed</t>
+  </si>
+  <si>
+    <t>CtsCancerInfo</t>
+  </si>
+  <si>
+    <t>CtsLocation</t>
+  </si>
+  <si>
+    <t>CtsDrugTreatment</t>
+  </si>
+  <si>
+    <t>CtsTrialCustom</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>all|all|all|all|none|none</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>all|none|none</t>
+  </si>
+  <si>
+    <t>all|none|none|none</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>c3167|all|all|all|none|none</t>
+  </si>
+  <si>
+    <t>t:st</t>
+  </si>
+  <si>
+    <t>c4911|c147996|all|all|none|none</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=C3167&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=C4911&amp;st=C147996&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=C35850&amp;st=C150207&amp;stg=C6009&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=C9106&amp;st=C27819&amp;stg=C7508&amp;fin=C39877&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=99&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=paget+disease&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;va=1&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=4&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=1&amp;z=99501&amp;zp=200&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=2&amp;lcnty=United+States&amp;lst=NM&amp;lcty=Las+Cruces&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=3&amp;hos=Seattle+Cancer+Care+Alliance&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=prevention&amp;tt=screening&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;d=C2654&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;i=C65008&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=IV&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=NCI-2014-01340&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=Steven+A.+Rosenberg&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=Johns+Hopkins+University+%2F+Sidney+Kimmel+Cancer+Center&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?t=C4872&amp;st=C8287&amp;stg=C94774&amp;fin=C3036&amp;a=100&amp;q=tumor&amp;loc=2&amp;lcnty=Canada&amp;lcty=Toronto&amp;tt=treatment&amp;d=C287&amp;i=C15541&amp;tp=IV&amp;tid=NCI-0001&amp;in=Edwin+Choy&amp;lo=Alliance+for+Clinical+Trials+in+Oncology&amp;rl=2</t>
+  </si>
+  <si>
+    <t>t:st:stg</t>
+  </si>
+  <si>
+    <t>c35850|c150207|c6009|all|none|none</t>
+  </si>
+  <si>
+    <t>t:st:stg:fin</t>
+  </si>
+  <si>
+    <t>c9106|c27819|c7508|c39877|none|none</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>all|all|all|all|99|none</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>all|all|all|all|none|paget disease</t>
+  </si>
+  <si>
+    <t>loc:va</t>
+  </si>
+  <si>
+    <t>all|va-only</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>at nih</t>
+  </si>
+  <si>
+    <t>loc:z:zp</t>
+  </si>
+  <si>
+    <t>zip|99501|200</t>
+  </si>
+  <si>
+    <t>loc:lcnty:lst:lcty</t>
+  </si>
+  <si>
+    <t>csc|united states|nm|las cruces</t>
+  </si>
+  <si>
+    <t>loc:hos</t>
+  </si>
+  <si>
+    <t>hi|seattle cancer care alliance</t>
+  </si>
+  <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>pre,scr|none|none</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>all|c2654|none</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>all|none|c65008</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+  <si>
+    <t>iv|none|none|none</t>
+  </si>
+  <si>
+    <t>tid</t>
+  </si>
+  <si>
+    <t>all|single:nci-2014-01340|none|none</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>all|none|steven a. rosenberg|none</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>all|none|none|johns hopkins university / sidney kimmel cancer center</t>
+  </si>
+  <si>
+    <t>t:st:stg:fin:a:q:loc:lcnty:lcty:tt:d:i:tp:tid:in:lo</t>
+  </si>
+  <si>
+    <t>c4872|c8287|c94774|c3036|100|tumor</t>
+  </si>
+  <si>
+    <t>csc|canada|none|toronto</t>
+  </si>
+  <si>
+    <t>tre|c287|c15541</t>
+  </si>
+  <si>
+    <t>iv|single:nci-0001|edwin choy|alliance for clinical trials in oncology</t>
   </si>
 </sst>
 </file>
@@ -444,11 +725,557 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6580A5B9-FE60-4431-8155-10501A984634}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B30AA94-7E47-4857-A53C-1EE50BAC543D}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cleaned up BasicResultsLoad test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-cts.xlsx
+++ b/test-data/webanalytics-cts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1DC2209E-C06F-4FEB-8D03-CB5930E1230A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DB38196-38C1-48F1-9F10-190E03AA2013}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="158">
   <si>
     <t>Path</t>
   </si>
@@ -360,6 +360,147 @@
   </si>
   <si>
     <t>iv|single:nci-0001|edwin choy|alliance for clinical trials in oncology</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Keyword/Age/Zip</t>
+  </si>
+  <si>
+    <t>Cancer Type/Zip</t>
+  </si>
+  <si>
+    <t>Cancer Type/Age</t>
+  </si>
+  <si>
+    <t>Keyword/Age</t>
+  </si>
+  <si>
+    <t>Keyword/Zip</t>
+  </si>
+  <si>
+    <t>?q=&amp;t=&amp;a=&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?t=C9087&amp;a=&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?q=medulla&amp;t=&amp;a=&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?q=&amp;t=&amp;a=80&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?q=&amp;t=&amp;a=&amp;z=20772&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?t=C3869&amp;a=85&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?q=androgen&amp;t=&amp;a=&amp;z=25063&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?t=C3242&amp;a=101&amp;z=96795&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?q=plasma&amp;t=&amp;a=70&amp;z=60044&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?t=&amp;a=age&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>?q=&amp;t=&amp;a=&amp;z=abcd&amp;rl=1</t>
+  </si>
+  <si>
+    <t>Cancer Type/Age/Zip</t>
+  </si>
+  <si>
+    <t>?q=Interstitial+&amp;t=&amp;a=78&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>?t=C7853&amp;a=&amp;z=29401&amp;rl=1</t>
+  </si>
+  <si>
+    <t>none|none</t>
+  </si>
+  <si>
+    <t>typecondition|c9087|none</t>
+  </si>
+  <si>
+    <t>keyword|medulla|none</t>
+  </si>
+  <si>
+    <t>none|80</t>
+  </si>
+  <si>
+    <t>loc:z</t>
+  </si>
+  <si>
+    <t>zip|20772|none</t>
+  </si>
+  <si>
+    <t>t:a</t>
+  </si>
+  <si>
+    <t>typecondition|c3869|85</t>
+  </si>
+  <si>
+    <t>q:loc:z</t>
+  </si>
+  <si>
+    <t>keyword|androgen|none</t>
+  </si>
+  <si>
+    <t>zip|25063|none</t>
+  </si>
+  <si>
+    <t>t:a:loc:z</t>
+  </si>
+  <si>
+    <t>typecondition|c3242|101</t>
+  </si>
+  <si>
+    <t>zip|96795|none</t>
+  </si>
+  <si>
+    <t>a:q:loc:z</t>
+  </si>
+  <si>
+    <t>keyword|plasma|70</t>
+  </si>
+  <si>
+    <t>zip|60044|none</t>
+  </si>
+  <si>
+    <t>zip|none|none</t>
+  </si>
+  <si>
+    <t>t:loc:z</t>
+  </si>
+  <si>
+    <t>zip|29401|none</t>
+  </si>
+  <si>
+    <t>typecondition|c7853|none</t>
+  </si>
+  <si>
+    <t>a:q</t>
+  </si>
+  <si>
+    <t>keyword|interstitial|78</t>
+  </si>
+  <si>
+    <t>All Trials (no params)</t>
+  </si>
+  <si>
+    <t>Invalid (age)</t>
+  </si>
+  <si>
+    <t>Invalid (zip)</t>
+  </si>
+  <si>
+    <t>?q=&amp;t=&amp;a=500&amp;z=&amp;rl=1</t>
   </si>
 </sst>
 </file>
@@ -726,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6580A5B9-FE60-4431-8155-10501A984634}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,9 +878,9 @@
     <col min="1" max="1" width="83" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1224,6 +1365,29 @@
       </c>
       <c r="G21" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1233,19 +1397,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B30AA94-7E47-4857-A53C-1EE50BAC543D}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,6 +1427,244 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up TrialDetailViewLoad test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-cts.xlsx
+++ b/test-data/webanalytics-cts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6314C709-BE7B-44D1-99F7-6F05C9233772}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{732E3F21-5477-451D-AAD9-755F1BFE763C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdvancedResultsLoad" sheetId="10" r:id="rId1"/>
     <sheet name="BasicResultsLoad" sheetId="11" r:id="rId2"/>
     <sheet name="DynamicListingPage" sheetId="9" r:id="rId3"/>
+    <sheet name="TrialDetailView" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,11 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="165">
   <si>
     <t>Path</t>
   </si>
   <si>
+    <t>ContentType</t>
+  </si>
+  <si>
     <t>/about-cancer/treatment/clinical-trials/disease/breast-cancer</t>
   </si>
   <si>
@@ -501,6 +505,24 @@
   </si>
   <si>
     <t>ListingType</t>
+  </si>
+  <si>
+    <t>?t=C4911&amp;q=nivolumab&amp;loc=0&amp;tid=S1609&amp;rl=2&amp;id=NCI-2016-01041&amp;pn=1&amp;ni=10</t>
+  </si>
+  <si>
+    <t>?q=ipilimumab&amp;loc=1&amp;z=20850&amp;zp=100&amp;rl=1&amp;id=NCI-2016-01041&amp;pn=1&amp;ni=10</t>
+  </si>
+  <si>
+    <t>?id=NCI-2016-01041&amp;r=1</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -886,508 +908,508 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
         <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1414,257 +1436,257 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
         <v>150</v>
-      </c>
-      <c r="E10" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1676,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150F8A41-7261-4E53-BBD5-6BBEA8E99D53}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,76 +1714,127 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E37697-AE5B-4CE3-B48B-AD53CE3285B3}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>